<commit_message>
End instruction. Remove date protector
</commit_message>
<xml_diff>
--- a/Лист Microsoft Excel.xlsx
+++ b/Лист Microsoft Excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>status_5_date</t>
+  </si>
+  <si>
+    <t>Поступил на склад в Китай.</t>
+  </si>
+  <si>
+    <t>4565</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1109,6 +1115,56 @@
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>456</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>6</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>